<commit_message>
Update Slack jobs Excel: 2025-06-24T18:48:50.836898
</commit_message>
<xml_diff>
--- a/slack apo.xlsx
+++ b/slack apo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,19 +475,11 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>tel:07777497199|07777497199</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>046</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>&lt;tel:07777497199|07777497199&gt; job no 0000002 pick up from, office station yard going to zest of India. Card failed in car owes Drv 046 £15</t>
-        </is>
-      </c>
+          <t>0785972311</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>U092FMBAUP7</t>
@@ -495,28 +487,28 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>&lt;tel:07777497199|07777497199&gt; job no 0000002 pick up from, office station yard going to zest of India. Card failed in car owes Drv 046 £15</t>
+          <t>0785972311 job no 7896541 pick up zest of india to, office owes 311 £18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>07777497162</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>07777497162</t>
+          <t>tel:07777497199|07777497199</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>046</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>&lt;tel:07777497199|07777497199&gt; job no 0000002 pick up from, office station yard going to zest of India. Card failed in car owes Drv 046 £15</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>U092FMBAUP7</t>
@@ -524,24 +516,28 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>07777497162 job no 000001 went from 2 primrose close -&amp;gt; tesco. Owes £5 to drv 100</t>
+          <t>&lt;tel:07777497199|07777497199&gt; job no 0000002 pick up from, office station yard going to zest of India. Card failed in car owes Drv 046 £15</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>07777497162</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0789456123</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0789456123 owes 102 £90 card failed on the app. Office and went to Manchester airport job num 12344567</t>
-        </is>
-      </c>
+          <t>07777497162</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>U092FMBAUP7</t>
@@ -549,30 +545,22 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0789456123 owes 102 £90 card failed on the app. Office and went to Manchester airport job num 12344567</t>
+          <t>07777497162 job no 000001 went from 2 primrose close -&amp;gt; tesco. Owes £5 to drv 100</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>07857896002</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>07857896002</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>143</t>
-        </is>
-      </c>
+          <t>0789456123</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>07857896002 owes drv 143 £8.99 card failed in car job num 78965432 new card not been activated so could not pay</t>
+          <t>0789456123 owes 102 £90 card failed on the app. Office and went to Manchester airport job num 12344567</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -582,7 +570,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>07857896002 owes drv 143 £8.99 card failed in car job num 78965432 new card not been activated so could not pay</t>
+          <t>0789456123 owes 102 £90 card failed on the app. Office and went to Manchester airport job num 12344567</t>
         </is>
       </c>
     </row>
@@ -590,41 +578,45 @@
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
+          <t>07857896002</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>07857896002</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>07857896002 owes drv 143 £8.99 card failed in car job num 78965432 new card not been activated so could not pay</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>U092FMBAUP7</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>07857896002 owes drv 143 £8.99 card failed in car job num 78965432 new card not been activated so could not pay</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>07840851310</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>314</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>U092FMBAUP7</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Chris at 314 Clifton drive north owes 091 £6.10 (said he would come in and pay £10 next week). 314 Clifton Drive North to Alexandria Pharmacy W/R *73278058 07840851310 -* If not in by next Friday please chase.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>68717887</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>07729772678</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>07729772678</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -636,32 +628,36 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>Chris at 314 Clifton drive north owes 091 £6.10 (said he would come in and pay £10 next week). 314 Clifton Drive North to Alexandria Pharmacy W/R *73278058 07840851310 -* If not in by next Friday please chase.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>68717887</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>07729772678</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>07729772678</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>U092FMBAUP7</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>*07729772678 - paid £14.80 owed to 218 from 2023* JOB 68717887*- number unbarred. - driver informed (91 will be bringing cash into the office minus the card charge*</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>71968922</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>71968922 0777749716 owes 046 £5 card failed in car Joseph piced up from office going to 2 primrose close</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>U092FMBAUP7</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>71968922 0777749716 owes 046 £5 card failed in car Joseph piced up from office going to 2 primrose close</t>
         </is>
       </c>
     </row>
@@ -670,19 +666,23 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>@U092AM83RD4</t>
+          <t>71968922</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>71968922 0777749716 owes 046 £5 card failed in car Joseph piced up from office going to 2 primrose close</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>U092AM83RD4</t>
+          <t>U092FMBAUP7</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>&lt;@U092AM83RD4&gt; has joined the channel</t>
+          <t>71968922 0777749716 owes 046 £5 card failed in car Joseph piced up from office going to 2 primrose close</t>
         </is>
       </c>
     </row>
@@ -691,17 +691,38 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>@U092FMBAUP7</t>
+          <t>@U092AM83RD4</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>U092FMBAUP7</t>
+          <t>U092AM83RD4</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
+        <is>
+          <t>&lt;@U092AM83RD4&gt; has joined the channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>@U092FMBAUP7</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>U092FMBAUP7</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>&lt;@U092FMBAUP7&gt; has joined the channel</t>
         </is>

</xml_diff>

<commit_message>
Update Slack jobs Excel: 2025-06-25T11:01:02.220019
</commit_message>
<xml_diff>
--- a/slack apo.xlsx
+++ b/slack apo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,15 +467,43 @@
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>07777497166</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>07777497166</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>046</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>07777497166 job no 7849325 Pick up at 2 Primrose close, going to office station yard. owes drv 046 £25 Card failed in the car said he will pay in a few days</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>U092FMBAUP7</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>0785972311</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>U092FMBAUP7</t>
         </is>

</xml_diff>